<commit_message>
events.xlsx; data; Starts adding overheat event
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">pathString</t>
   </si>
@@ -64,16 +64,31 @@
     <t xml:space="preserve">package</t>
   </si>
   <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">events/nothing</t>
   </si>
   <si>
     <t xml:space="preserve">function(ship,node,...){   sample(c("Deep in space, the AI wakes suddenly to an alert from the medical monitoring program. It anxiously checks the colonists, but finds that there is no problem, and the alert was a glitch. Nevertheless, the AI spends some time watching its sleeping charges, reassuring itself that they are all alive, before it joins them again in sleep."     ,"The AI is woken from its hibernation by a possible malfunction warning, but a systems check reveals that it was a false alarm. Far from the nearest star, the AI spends some time admiring the cold beauty of the Milky Way as revealed by its navigation sensors, before returning to hibernation to wait for its arrival in the next system."     ,"The next star chosen by the guidance system is on the other side of a great void, with no stars for dozens of light years. The AI hibernates for the millennia-long journey through utter emptiness."     ,"For centuries the seedship drifts towards its next destination, very nearly inert, the AI hibernating and only the simple collision avoidance and damage monitoring systems ticking over."     ,"The seedship's course takes it through a dense star cluster, and while the AI sleeps the guidance system weaves a complex course through the stars' overlapping gravitational fields."),1) }</t>
   </si>
   <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
     <t xml:space="preserve">events/overheat</t>
   </si>
   <si>
-    <t xml:space="preserve">Overheat!</t>
+    <t xml:space="preserve">The AI wakes to a wall of blinding brightness. The seedship's course has taken it close to a super-giant star that has proved to be far hotter than the guidance system anticipated, and the ship is gathering heat faster than the radiator fins can radiate it away. The AI must shut down part of the heat regulation system before the entire system catastrophically fails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overheat/colonists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow the sleep chambers to overheat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI channels excess heat into the sleep chambers. The heat regulation system recovers as the ship moves away from the super-hot star, but not before [?-75] colonists have sustained tissue damage too severe for them to be successfully revived.</t>
   </si>
 </sst>
 </file>
@@ -83,11 +98,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,6 +119,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,9 +168,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -169,93 +202,116 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="296.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>15</v>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="0" t="n">
+    <row r="3" customFormat="false" ht="152.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="106.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functions.R; bugfix; Fixes inappropriate damage bug in navigateEvent(). Corrects data source for events in a few places. Adds autoadvance feature-- if a node has only one child node and autoadvance is TRUE, do not prompt player to advance.
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">pathString</t>
   </si>
@@ -89,6 +89,45 @@
   </si>
   <si>
     <t xml:space="preserve">The AI channels excess heat into the sleep chambers. The heat regulation system recovers as the ship moves away from the super-hot star, but not before [?-75] colonists have sustained tissue damage too severe for them to be successfully revived.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_systems=1, max_damage=75,damageable="colonists"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overheat/scanner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow the scanner module to overheat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI channels excess heat into the scanner array. The heat regulation system recovers as the ship moves away from the super-hot star, but not before the heat has damaged a scanner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_systems=1, max_damage=15,damageable=c("resources_sensor","temperature_sensor", "gravity_sensor", "atmosphere_sensor","water_sensor")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overheat/gearlanding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow the landing/construction module to overheat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI channels excess heat into the landing gear and construction equipment. The heat regulation system recovers as the ship moves away from the super-hot star, but not before some heat damage is done.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_systems=1, max_damage=2,damageable=c("landing_gear","equipment")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overheat/dbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow the data storage module to overheat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI channels excess heat into the data storage module. The heat regulation system recovers as the ship moves away from the super-hot star, but not before some data is lost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_systems=1, max_damage=7,damageable=c("planetLocalDB","dbase")</t>
   </si>
 </sst>
 </file>
@@ -168,7 +207,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,8 +216,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -202,16 +245,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.95"/>
@@ -229,7 +272,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -268,7 +311,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -299,18 +342,74 @@
       <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="106.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F4" s="0"/>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="L4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
events.xlsx; events; Adds radiation and overwhelmed.
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t xml:space="preserve">pathString</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">dynchoices</t>
   </si>
   <si>
+    <t xml:space="preserve">autoadvance</t>
+  </si>
+  <si>
     <t xml:space="preserve">package</t>
   </si>
   <si>
@@ -79,9 +82,15 @@
     <t xml:space="preserve">events/overheat</t>
   </si>
   <si>
+    <t xml:space="preserve">function(ship,node,...){prepStarChart(ship) %&gt;% subset(distance &lt; 1) %&gt;% nrow()}</t>
+  </si>
+  <si>
     <t xml:space="preserve">The AI wakes to a wall of blinding brightness. The seedship's course has taken it close to a super-giant star that has proved to be far hotter than the guidance system anticipated, and the ship is gathering heat faster than the radiator fins can radiate it away. The AI must shut down part of the heat regulation system before the entire system catastrophically fails.</t>
   </si>
   <si>
+    <t xml:space="preserve">Dynamic value dependent on number of nearby stars. Once we have actual star-systems, will depend on number of supergiants probably.</t>
+  </si>
+  <si>
     <t xml:space="preserve">events/overheat/colonists</t>
   </si>
   <si>
@@ -94,7 +103,7 @@
     <t xml:space="preserve">max_systems=1, max_damage=75,damageable="colonists"</t>
   </si>
   <si>
-    <t xml:space="preserve">events/overheat/scanner</t>
+    <t xml:space="preserve">events/overheat/sensors</t>
   </si>
   <si>
     <t xml:space="preserve">Allow the scanner module to overheat</t>
@@ -103,10 +112,10 @@
     <t xml:space="preserve">The AI channels excess heat into the scanner array. The heat regulation system recovers as the ship moves away from the super-hot star, but not before the heat has damaged a scanner.</t>
   </si>
   <si>
-    <t xml:space="preserve">max_systems=1, max_damage=15,damageable=c("resources_sensor","temperature_sensor", "gravity_sensor", "atmosphere_sensor","water_sensor")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">events/overheat/gearlanding</t>
+    <t xml:space="preserve">max_systems=1, max_damage=15,damageable="sensors"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overheat/lgeq</t>
   </si>
   <si>
     <t xml:space="preserve">Allow the landing/construction module to overheat</t>
@@ -115,10 +124,10 @@
     <t xml:space="preserve">The AI channels excess heat into the landing gear and construction equipment. The heat regulation system recovers as the ship moves away from the super-hot star, but not before some heat damage is done.</t>
   </si>
   <si>
-    <t xml:space="preserve">max_systems=1, max_damage=2,damageable=c("landing_gear","equipment")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">events/overheat/dbase</t>
+    <t xml:space="preserve">max_systems=1, max_damage=2,damageable="lgeq"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overheat/dbs</t>
   </si>
   <si>
     <t xml:space="preserve">Allow the data storage module to overheat</t>
@@ -127,15 +136,113 @@
     <t xml:space="preserve">The AI channels excess heat into the data storage module. The heat regulation system recovers as the ship moves away from the super-hot star, but not before some data is lost.</t>
   </si>
   <si>
-    <t xml:space="preserve">max_systems=1, max_damage=7,damageable=c("planetLocalDB","dbase")</t>
+    <t xml:space="preserve">max_systems=1, max_damage=7,damageable="dbs"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI wakes to a radiation alert: the death burst of a distant supernova is flooding the seedship's electronics with random signals. The ${ship$eventcache$radiation} is malfunctioning, and in a few moments it will be permanently damaged. The seedship could avoid the malfunction by shutting down all its electronics until the radiation has passed, but that would leave it without a working collision avoidance system for a dangerous length of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function(ship,node,...){radsystem  &lt;- sample(c("scanners","lgeq","dbs"),1); list(eventcache=list(radiation=sample(names(getShipNumericStats(ship,radsystem)),1)))}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/radiation/shutdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shut down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI shuts down all the ship's systems and then itself. When it comes back online the radiation has passed…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/radiation/shutdown/nodamage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">...and to its relief a systems check reveals no damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/radiation/shutdown/damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">...but a small asteroid has torn a hole in the ${names(damaged)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_systems=1, max_damage=30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/radiation/noshutdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't shut down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI keeps its focus on the collision avoidance system while radiation wrecks delicate components deep in the ${names(damaged)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function(ship,node,...){list(shipstats=list(max_systems=1,min_damage=10,max_damage=15,damageable=ship$eventcache$radiation))}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overwhelmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function(ship,node,...){prepStarChart(ship) %&gt;% subset(distance &lt; 7) %&gt;% nrow() }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The seedship's course takes it through a dense star-forming nebula. Hundreds of infant suns illuminate clouds of interstellar gas and fill the sky with riotous color. Clouds twist through complex gravitational interference patterns and glitter with heavy elements formed in the death throes of the last generation of stars. 
+The scanners were not designed to deal with this level of input, and it is threatening to overwhelm them. If the AI continues to use the scanners to navigate, it can tell that the ${ship$eventcache$overwhelmed} will be damaged. Shutting off the scanners, however, would leave the seedship vulnerable to collisions in this crowded area of space.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function(ship,node,...){list(eventcache=list(overwhelmed=sample(names(getShipNumericStats(ship,'sensors')),1)))}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO: only allow non-destroyed scanners to get overwhelmed, and handle the case where there are no working scanners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overwhelmed/runscanners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep the scanners running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI continues to use the scanners to navigate. The ${ship$eventcache$overwhelmed} overloads, but the seedship passes safely through the star-forming nebula.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function(ship,node,...){list(shipstats=list(max_systems=1,min_damage=15,max_damage=35,damageable=ship$eventcache$overwhelmed))}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overwhelmed/flyblind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly blind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The AI calculates a course that it thinks will avoid obstacles, then shuts down the scanners.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overwhelmed/flyblind/nodamage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To it's relief, when it judges that it is out of danger and reactivates the scanners, there is no damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">events/overwhelmed/flyblind/damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flying blind, it has no way of detecting the dense cloud of dust that buffets the ship and wears away at ${paste0(names(damaged),collapse=", ")}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_damage=12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -207,7 +314,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +335,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,10 +360,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -265,10 +380,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="8.39"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -314,103 +429,316 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="152.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="106.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0"/>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L5" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L6" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="19.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L7" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>